<commit_message>
login credentials along with Role has been added
</commit_message>
<xml_diff>
--- a/stepFiles/Login.xlsx
+++ b/stepFiles/Login.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/naveenupputuri/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/naveenupputuri/eclipse-workspace/testcucumber/stepFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A87A9D05-CDB5-6741-8CCE-52B338CAD5E9}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5D65723-A463-614F-8A06-F5AA5585E375}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16460" xr2:uid="{8D2098BF-096D-9B48-B995-EEF419F7D40E}"/>
+    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16420" xr2:uid="{8D2098BF-096D-9B48-B995-EEF419F7D40E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -45,22 +45,22 @@
     <t>SDET</t>
   </si>
   <si>
-    <t>upputuri.naveen01</t>
+    <t>upputui.naveen01</t>
   </si>
   <si>
     <t>Unaveen9#</t>
   </si>
   <si>
+    <t>naveen.amfg26</t>
+  </si>
+  <si>
+    <t>upputuri1990</t>
+  </si>
+  <si>
     <t>QA LEAD</t>
   </si>
   <si>
-    <t>naveen.amfg26</t>
-  </si>
-  <si>
-    <t>upputuri1990</t>
-  </si>
-  <si>
-    <t>Manager</t>
+    <t>team lead</t>
   </si>
 </sst>
 </file>
@@ -415,7 +415,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -450,18 +450,18 @@
         <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
         <v>9</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>10</v>
-      </c>
-      <c r="C4" t="s">
-        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>